<commit_message>
Updated geocoding script to write to text and pickle files.
</commit_message>
<xml_diff>
--- a/xslx/Geocoder Test Suite - Final.xlsx
+++ b/xslx/Geocoder Test Suite - Final.xlsx
@@ -16,10 +16,9 @@
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$Q$1740</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$Q$1739</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13792" uniqueCount="2448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13686" uniqueCount="2447">
   <si>
     <t>Type</t>
   </si>
@@ -7325,9 +7324,6 @@
   </si>
   <si>
     <t>User Selected</t>
-  </si>
-  <si>
-    <t>E 8th Street &amp; Main</t>
   </si>
   <si>
     <t>Hilton Vancouver Washington</t>
@@ -8884,10 +8880,10 @@
     </row>
     <row r="13" spans="1:27" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>2445</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>2446</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>2447</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>2085</v>
@@ -8913,11 +8909,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1740"/>
+  <dimension ref="A1:R1739"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A460" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C492" sqref="C492"/>
+      <pane ySplit="1" topLeftCell="A1557" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1568" sqref="G1568"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -80012,9 +80008,7 @@
         <v>2200</v>
       </c>
       <c r="F1566" s="2"/>
-      <c r="G1566" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1566" s="2"/>
       <c r="H1566" s="2" t="s">
         <v>1878</v>
       </c>
@@ -80063,9 +80057,7 @@
         <v>2201</v>
       </c>
       <c r="F1567" s="2"/>
-      <c r="G1567" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1567" s="2"/>
       <c r="H1567" s="2" t="s">
         <v>144</v>
       </c>
@@ -80114,9 +80106,7 @@
         <v>2202</v>
       </c>
       <c r="F1568" s="2"/>
-      <c r="G1568" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1568" s="2"/>
       <c r="H1568" s="2" t="s">
         <v>2157</v>
       </c>
@@ -80165,9 +80155,7 @@
         <v>2203</v>
       </c>
       <c r="F1569" s="2"/>
-      <c r="G1569" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1569" s="2"/>
       <c r="H1569" s="2" t="s">
         <v>643</v>
       </c>
@@ -80216,9 +80204,7 @@
         <v>2204</v>
       </c>
       <c r="F1570" s="2"/>
-      <c r="G1570" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1570" s="2"/>
       <c r="H1570" s="2" t="s">
         <v>369</v>
       </c>
@@ -80267,9 +80253,7 @@
         <v>2205</v>
       </c>
       <c r="F1571" s="2"/>
-      <c r="G1571" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1571" s="2"/>
       <c r="H1571" s="2" t="s">
         <v>2158</v>
       </c>
@@ -80318,9 +80302,7 @@
         <v>2228</v>
       </c>
       <c r="F1572" s="2"/>
-      <c r="G1572" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1572" s="2"/>
       <c r="H1572" s="2" t="s">
         <v>2157</v>
       </c>
@@ -80369,9 +80351,7 @@
         <v>2206</v>
       </c>
       <c r="F1573" s="2"/>
-      <c r="G1573" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1573" s="2"/>
       <c r="H1573" s="2" t="s">
         <v>2159</v>
       </c>
@@ -80420,9 +80400,7 @@
         <v>2207</v>
       </c>
       <c r="F1574" s="2"/>
-      <c r="G1574" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1574" s="2"/>
       <c r="H1574" s="2" t="s">
         <v>1270</v>
       </c>
@@ -80471,9 +80449,7 @@
         <v>2208</v>
       </c>
       <c r="F1575" s="2"/>
-      <c r="G1575" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1575" s="2"/>
       <c r="H1575" s="2" t="s">
         <v>144</v>
       </c>
@@ -80522,9 +80498,7 @@
         <v>2209</v>
       </c>
       <c r="F1576" s="2"/>
-      <c r="G1576" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1576" s="2"/>
       <c r="H1576" s="2" t="s">
         <v>643</v>
       </c>
@@ -80573,9 +80547,7 @@
         <v>2210</v>
       </c>
       <c r="F1577" s="2"/>
-      <c r="G1577" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1577" s="2"/>
       <c r="H1577" s="2" t="s">
         <v>2159</v>
       </c>
@@ -80624,9 +80596,7 @@
         <v>2211</v>
       </c>
       <c r="F1578" s="2"/>
-      <c r="G1578" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1578" s="2"/>
       <c r="H1578" s="2" t="s">
         <v>2160</v>
       </c>
@@ -80675,9 +80645,7 @@
         <v>2212</v>
       </c>
       <c r="F1579" s="2"/>
-      <c r="G1579" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1579" s="2"/>
       <c r="H1579" s="2" t="s">
         <v>2160</v>
       </c>
@@ -80726,9 +80694,7 @@
         <v>2213</v>
       </c>
       <c r="F1580" s="2"/>
-      <c r="G1580" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1580" s="2"/>
       <c r="H1580" s="2" t="s">
         <v>2157</v>
       </c>
@@ -80777,9 +80743,7 @@
         <v>2214</v>
       </c>
       <c r="F1581" s="2"/>
-      <c r="G1581" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1581" s="2"/>
       <c r="H1581" s="2" t="s">
         <v>2161</v>
       </c>
@@ -80828,9 +80792,7 @@
         <v>2221</v>
       </c>
       <c r="F1582" s="2"/>
-      <c r="G1582" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1582" s="2"/>
       <c r="H1582" s="2" t="s">
         <v>2162</v>
       </c>
@@ -80879,9 +80841,7 @@
         <v>2215</v>
       </c>
       <c r="F1583" s="2"/>
-      <c r="G1583" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1583" s="2"/>
       <c r="H1583" s="2" t="s">
         <v>783</v>
       </c>
@@ -80930,9 +80890,7 @@
         <v>2216</v>
       </c>
       <c r="F1584" s="2"/>
-      <c r="G1584" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1584" s="2"/>
       <c r="H1584" s="2" t="s">
         <v>2159</v>
       </c>
@@ -80981,9 +80939,7 @@
         <v>2217</v>
       </c>
       <c r="F1585" s="2"/>
-      <c r="G1585" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1585" s="2"/>
       <c r="H1585" s="2" t="s">
         <v>2159</v>
       </c>
@@ -81032,9 +80988,7 @@
         <v>2218</v>
       </c>
       <c r="F1586" s="2"/>
-      <c r="G1586" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1586" s="2"/>
       <c r="H1586" s="2" t="s">
         <v>2159</v>
       </c>
@@ -81083,9 +81037,7 @@
         <v>2219</v>
       </c>
       <c r="F1587" s="2"/>
-      <c r="G1587" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1587" s="2"/>
       <c r="H1587" s="2" t="s">
         <v>440</v>
       </c>
@@ -81134,9 +81086,7 @@
         <v>2220</v>
       </c>
       <c r="F1588" s="2"/>
-      <c r="G1588" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1588" s="2"/>
       <c r="H1588" s="2" t="s">
         <v>2162</v>
       </c>
@@ -81185,9 +81135,7 @@
         <v>2244</v>
       </c>
       <c r="F1589" s="2"/>
-      <c r="G1589" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1589" s="2"/>
       <c r="H1589" s="2" t="s">
         <v>2160</v>
       </c>
@@ -81236,9 +81184,7 @@
         <v>2221</v>
       </c>
       <c r="F1590" s="2"/>
-      <c r="G1590" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1590" s="2"/>
       <c r="H1590" s="2" t="s">
         <v>2162</v>
       </c>
@@ -81287,9 +81233,7 @@
         <v>2222</v>
       </c>
       <c r="F1591" s="2"/>
-      <c r="G1591" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1591" s="2"/>
       <c r="H1591" s="2" t="s">
         <v>2161</v>
       </c>
@@ -81338,9 +81282,7 @@
         <v>2223</v>
       </c>
       <c r="F1592" s="2"/>
-      <c r="G1592" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1592" s="2"/>
       <c r="H1592" s="2" t="s">
         <v>783</v>
       </c>
@@ -81389,9 +81331,7 @@
         <v>2214</v>
       </c>
       <c r="F1593" s="2"/>
-      <c r="G1593" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1593" s="2"/>
       <c r="H1593" s="2" t="s">
         <v>144</v>
       </c>
@@ -81440,9 +81380,7 @@
         <v>2208</v>
       </c>
       <c r="F1594" s="2"/>
-      <c r="G1594" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1594" s="2"/>
       <c r="H1594" s="2" t="s">
         <v>351</v>
       </c>
@@ -81491,9 +81429,7 @@
         <v>2224</v>
       </c>
       <c r="F1595" s="2"/>
-      <c r="G1595" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1595" s="2"/>
       <c r="H1595" s="2" t="s">
         <v>2163</v>
       </c>
@@ -81542,9 +81478,7 @@
         <v>2225</v>
       </c>
       <c r="F1596" s="2"/>
-      <c r="G1596" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1596" s="2"/>
       <c r="H1596" s="2" t="s">
         <v>144</v>
       </c>
@@ -81593,9 +81527,7 @@
         <v>2226</v>
       </c>
       <c r="F1597" s="2"/>
-      <c r="G1597" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1597" s="2"/>
       <c r="H1597" s="2" t="s">
         <v>2160</v>
       </c>
@@ -81644,9 +81576,7 @@
         <v>2227</v>
       </c>
       <c r="F1598" s="2"/>
-      <c r="G1598" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1598" s="2"/>
       <c r="H1598" s="2" t="s">
         <v>2163</v>
       </c>
@@ -81695,9 +81625,7 @@
         <v>2228</v>
       </c>
       <c r="F1599" s="2"/>
-      <c r="G1599" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1599" s="2"/>
       <c r="H1599" s="2" t="s">
         <v>2164</v>
       </c>
@@ -81746,9 +81674,7 @@
         <v>2229</v>
       </c>
       <c r="F1600" s="2"/>
-      <c r="G1600" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1600" s="2"/>
       <c r="H1600" s="2" t="s">
         <v>2159</v>
       </c>
@@ -81797,9 +81723,7 @@
         <v>2230</v>
       </c>
       <c r="F1601" s="2"/>
-      <c r="G1601" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1601" s="2"/>
       <c r="H1601" s="2" t="s">
         <v>2164</v>
       </c>
@@ -81848,9 +81772,7 @@
         <v>2417</v>
       </c>
       <c r="F1602" s="2"/>
-      <c r="G1602" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1602" s="2"/>
       <c r="H1602" s="2" t="s">
         <v>2165</v>
       </c>
@@ -81899,9 +81821,7 @@
         <v>2231</v>
       </c>
       <c r="F1603" s="2"/>
-      <c r="G1603" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1603" s="2"/>
       <c r="H1603" s="2" t="s">
         <v>144</v>
       </c>
@@ -81950,9 +81870,7 @@
         <v>2232</v>
       </c>
       <c r="F1604" s="2"/>
-      <c r="G1604" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1604" s="2"/>
       <c r="H1604" s="2" t="s">
         <v>643</v>
       </c>
@@ -82001,9 +81919,7 @@
         <v>2233</v>
       </c>
       <c r="F1605" s="2"/>
-      <c r="G1605" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1605" s="2"/>
       <c r="H1605" s="2" t="s">
         <v>2166</v>
       </c>
@@ -82052,9 +81968,7 @@
         <v>2234</v>
       </c>
       <c r="F1606" s="2"/>
-      <c r="G1606" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1606" s="2"/>
       <c r="H1606" s="2" t="s">
         <v>2167</v>
       </c>
@@ -82103,9 +82017,7 @@
         <v>2235</v>
       </c>
       <c r="F1607" s="2"/>
-      <c r="G1607" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1607" s="2"/>
       <c r="H1607" s="2" t="s">
         <v>2159</v>
       </c>
@@ -82154,9 +82066,7 @@
         <v>2236</v>
       </c>
       <c r="F1608" s="2"/>
-      <c r="G1608" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1608" s="2"/>
       <c r="H1608" s="2" t="s">
         <v>2164</v>
       </c>
@@ -82205,9 +82115,7 @@
         <v>2237</v>
       </c>
       <c r="F1609" s="2"/>
-      <c r="G1609" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1609" s="2"/>
       <c r="H1609" s="2" t="s">
         <v>1424</v>
       </c>
@@ -82256,9 +82164,7 @@
         <v>2238</v>
       </c>
       <c r="F1610" s="2"/>
-      <c r="G1610" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1610" s="2"/>
       <c r="H1610" s="2" t="s">
         <v>2159</v>
       </c>
@@ -82307,9 +82213,7 @@
         <v>2239</v>
       </c>
       <c r="F1611" s="2"/>
-      <c r="G1611" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1611" s="2"/>
       <c r="H1611" s="2" t="s">
         <v>783</v>
       </c>
@@ -82358,9 +82262,7 @@
         <v>2240</v>
       </c>
       <c r="F1612" s="2"/>
-      <c r="G1612" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1612" s="2"/>
       <c r="H1612" s="2" t="s">
         <v>440</v>
       </c>
@@ -82409,9 +82311,7 @@
         <v>2241</v>
       </c>
       <c r="F1613" s="2"/>
-      <c r="G1613" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1613" s="2"/>
       <c r="H1613" s="2" t="s">
         <v>398</v>
       </c>
@@ -82460,9 +82360,7 @@
         <v>2242</v>
       </c>
       <c r="F1614" s="2"/>
-      <c r="G1614" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1614" s="2"/>
       <c r="H1614" s="2" t="s">
         <v>2159</v>
       </c>
@@ -82511,9 +82409,7 @@
         <v>2243</v>
       </c>
       <c r="F1615" s="2"/>
-      <c r="G1615" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1615" s="2"/>
       <c r="H1615" s="2" t="s">
         <v>144</v>
       </c>
@@ -82562,9 +82458,7 @@
         <v>2244</v>
       </c>
       <c r="F1616" s="2"/>
-      <c r="G1616" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1616" s="2"/>
       <c r="H1616" s="2" t="s">
         <v>2164</v>
       </c>
@@ -82613,9 +82507,7 @@
         <v>2245</v>
       </c>
       <c r="F1617" s="2"/>
-      <c r="G1617" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1617" s="2"/>
       <c r="H1617" s="2" t="s">
         <v>1270</v>
       </c>
@@ -82664,9 +82556,7 @@
         <v>2246</v>
       </c>
       <c r="F1618" s="2"/>
-      <c r="G1618" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1618" s="2"/>
       <c r="H1618" s="2" t="s">
         <v>2168</v>
       </c>
@@ -82715,9 +82605,7 @@
         <v>2247</v>
       </c>
       <c r="F1619" s="2"/>
-      <c r="G1619" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1619" s="2"/>
       <c r="H1619" s="2" t="s">
         <v>2157</v>
       </c>
@@ -82766,9 +82654,7 @@
         <v>2421</v>
       </c>
       <c r="F1620" s="2"/>
-      <c r="G1620" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1620" s="2"/>
       <c r="H1620" s="2" t="s">
         <v>176</v>
       </c>
@@ -82817,9 +82703,7 @@
         <v>2248</v>
       </c>
       <c r="F1621" s="2"/>
-      <c r="G1621" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1621" s="2"/>
       <c r="H1621" s="2" t="s">
         <v>2159</v>
       </c>
@@ -82868,9 +82752,7 @@
         <v>2249</v>
       </c>
       <c r="F1622" s="2"/>
-      <c r="G1622" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1622" s="2"/>
       <c r="H1622" s="2" t="s">
         <v>2157</v>
       </c>
@@ -82919,9 +82801,7 @@
         <v>2250</v>
       </c>
       <c r="F1623" s="2"/>
-      <c r="G1623" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1623" s="2"/>
       <c r="H1623" s="2" t="s">
         <v>2161</v>
       </c>
@@ -82970,9 +82850,7 @@
         <v>2251</v>
       </c>
       <c r="F1624" s="2"/>
-      <c r="G1624" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1624" s="2"/>
       <c r="H1624" s="2" t="s">
         <v>2169</v>
       </c>
@@ -83021,9 +82899,7 @@
         <v>2252</v>
       </c>
       <c r="F1625" s="2"/>
-      <c r="G1625" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1625" s="2"/>
       <c r="H1625" s="2" t="s">
         <v>2170</v>
       </c>
@@ -83072,9 +82948,7 @@
         <v>2253</v>
       </c>
       <c r="F1626" s="2"/>
-      <c r="G1626" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1626" s="2"/>
       <c r="H1626" s="2" t="s">
         <v>2157</v>
       </c>
@@ -83123,9 +82997,7 @@
         <v>2254</v>
       </c>
       <c r="F1627" s="2"/>
-      <c r="G1627" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1627" s="2"/>
       <c r="H1627" s="2" t="s">
         <v>2159</v>
       </c>
@@ -83174,9 +83046,7 @@
         <v>2255</v>
       </c>
       <c r="F1628" s="2"/>
-      <c r="G1628" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1628" s="2"/>
       <c r="H1628" s="2" t="s">
         <v>398</v>
       </c>
@@ -83225,9 +83095,7 @@
         <v>2256</v>
       </c>
       <c r="F1629" s="2"/>
-      <c r="G1629" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1629" s="2"/>
       <c r="H1629" s="2" t="s">
         <v>2171</v>
       </c>
@@ -83276,9 +83144,7 @@
         <v>2257</v>
       </c>
       <c r="F1630" s="2"/>
-      <c r="G1630" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1630" s="2"/>
       <c r="H1630" s="2" t="s">
         <v>1270</v>
       </c>
@@ -83327,9 +83193,7 @@
         <v>2258</v>
       </c>
       <c r="F1631" s="2"/>
-      <c r="G1631" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1631" s="2"/>
       <c r="H1631" s="2" t="s">
         <v>440</v>
       </c>
@@ -83378,9 +83242,7 @@
         <v>2259</v>
       </c>
       <c r="F1632" s="2"/>
-      <c r="G1632" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1632" s="2"/>
       <c r="H1632" s="2" t="s">
         <v>1270</v>
       </c>
@@ -83429,9 +83291,7 @@
         <v>2418</v>
       </c>
       <c r="F1633" s="2"/>
-      <c r="G1633" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1633" s="2"/>
       <c r="H1633" s="2" t="s">
         <v>2157</v>
       </c>
@@ -83480,9 +83340,7 @@
         <v>2260</v>
       </c>
       <c r="F1634" s="2"/>
-      <c r="G1634" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1634" s="2"/>
       <c r="H1634" s="2" t="s">
         <v>2163</v>
       </c>
@@ -83531,9 +83389,7 @@
         <v>2261</v>
       </c>
       <c r="F1635" s="2"/>
-      <c r="G1635" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1635" s="2"/>
       <c r="H1635" s="2" t="s">
         <v>942</v>
       </c>
@@ -83582,9 +83438,7 @@
         <v>2262</v>
       </c>
       <c r="F1636" s="2"/>
-      <c r="G1636" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1636" s="2"/>
       <c r="H1636" s="2" t="s">
         <v>2163</v>
       </c>
@@ -83633,9 +83487,7 @@
         <v>2263</v>
       </c>
       <c r="F1637" s="2"/>
-      <c r="G1637" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1637" s="2"/>
       <c r="H1637" s="2" t="s">
         <v>144</v>
       </c>
@@ -83684,9 +83536,7 @@
         <v>2264</v>
       </c>
       <c r="F1638" s="2"/>
-      <c r="G1638" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1638" s="2"/>
       <c r="H1638" s="2" t="s">
         <v>2172</v>
       </c>
@@ -83735,9 +83585,7 @@
         <v>2265</v>
       </c>
       <c r="F1639" s="2"/>
-      <c r="G1639" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1639" s="2"/>
       <c r="H1639" s="2" t="s">
         <v>369</v>
       </c>
@@ -83786,9 +83634,7 @@
         <v>2266</v>
       </c>
       <c r="F1640" s="2"/>
-      <c r="G1640" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1640" s="2"/>
       <c r="H1640" s="2" t="s">
         <v>2162</v>
       </c>
@@ -83837,9 +83683,7 @@
         <v>2267</v>
       </c>
       <c r="F1641" s="2"/>
-      <c r="G1641" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1641" s="2"/>
       <c r="H1641" s="2" t="s">
         <v>2164</v>
       </c>
@@ -83888,9 +83732,7 @@
         <v>2268</v>
       </c>
       <c r="F1642" s="2"/>
-      <c r="G1642" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1642" s="2"/>
       <c r="H1642" s="2" t="s">
         <v>2161</v>
       </c>
@@ -83939,9 +83781,7 @@
         <v>2269</v>
       </c>
       <c r="F1643" s="2"/>
-      <c r="G1643" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1643" s="2"/>
       <c r="H1643" s="2" t="s">
         <v>144</v>
       </c>
@@ -83990,9 +83830,7 @@
         <v>2252</v>
       </c>
       <c r="F1644" s="2"/>
-      <c r="G1644" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1644" s="2"/>
       <c r="H1644" s="2" t="s">
         <v>2173</v>
       </c>
@@ -84041,9 +83879,7 @@
         <v>2270</v>
       </c>
       <c r="F1645" s="2"/>
-      <c r="G1645" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1645" s="2"/>
       <c r="H1645" s="2" t="s">
         <v>2163</v>
       </c>
@@ -84092,9 +83928,7 @@
         <v>2271</v>
       </c>
       <c r="F1646" s="2"/>
-      <c r="G1646" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1646" s="2"/>
       <c r="H1646" s="2" t="s">
         <v>2164</v>
       </c>
@@ -84143,9 +83977,7 @@
         <v>2272</v>
       </c>
       <c r="F1647" s="2"/>
-      <c r="G1647" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1647" s="2"/>
       <c r="H1647" s="2" t="s">
         <v>2164</v>
       </c>
@@ -84194,9 +84026,7 @@
         <v>2273</v>
       </c>
       <c r="F1648" s="2"/>
-      <c r="G1648" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1648" s="2"/>
       <c r="H1648" s="2" t="s">
         <v>2160</v>
       </c>
@@ -84245,9 +84075,7 @@
         <v>2274</v>
       </c>
       <c r="F1649" s="2"/>
-      <c r="G1649" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1649" s="2"/>
       <c r="H1649" s="2" t="s">
         <v>2164</v>
       </c>
@@ -84296,9 +84124,7 @@
         <v>2275</v>
       </c>
       <c r="F1650" s="2"/>
-      <c r="G1650" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1650" s="2"/>
       <c r="H1650" s="2" t="s">
         <v>144</v>
       </c>
@@ -84347,9 +84173,7 @@
         <v>2276</v>
       </c>
       <c r="F1651" s="2"/>
-      <c r="G1651" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1651" s="2"/>
       <c r="H1651" s="2" t="s">
         <v>2157</v>
       </c>
@@ -84398,9 +84222,7 @@
         <v>2277</v>
       </c>
       <c r="F1652" s="2"/>
-      <c r="G1652" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1652" s="2"/>
       <c r="H1652" s="2" t="s">
         <v>2166</v>
       </c>
@@ -84449,9 +84271,7 @@
         <v>2266</v>
       </c>
       <c r="F1653" s="2"/>
-      <c r="G1653" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1653" s="2"/>
       <c r="H1653" s="2" t="s">
         <v>2159</v>
       </c>
@@ -84500,9 +84320,7 @@
         <v>2278</v>
       </c>
       <c r="F1654" s="2"/>
-      <c r="G1654" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1654" s="2"/>
       <c r="H1654" s="2" t="s">
         <v>2163</v>
       </c>
@@ -84551,9 +84369,7 @@
         <v>2279</v>
       </c>
       <c r="F1655" s="2"/>
-      <c r="G1655" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1655" s="2"/>
       <c r="H1655" s="2" t="s">
         <v>2160</v>
       </c>
@@ -84602,9 +84418,7 @@
         <v>2280</v>
       </c>
       <c r="F1656" s="2"/>
-      <c r="G1656" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1656" s="2"/>
       <c r="H1656" s="2" t="s">
         <v>2159</v>
       </c>
@@ -84653,9 +84467,7 @@
         <v>2225</v>
       </c>
       <c r="F1657" s="2"/>
-      <c r="G1657" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1657" s="2"/>
       <c r="H1657" s="2" t="s">
         <v>2162</v>
       </c>
@@ -84704,9 +84516,7 @@
         <v>2281</v>
       </c>
       <c r="F1658" s="2"/>
-      <c r="G1658" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1658" s="2"/>
       <c r="H1658" s="2" t="s">
         <v>2161</v>
       </c>
@@ -84755,9 +84565,7 @@
         <v>2282</v>
       </c>
       <c r="F1659" s="2"/>
-      <c r="G1659" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1659" s="2"/>
       <c r="H1659" s="2" t="s">
         <v>942</v>
       </c>
@@ -84806,9 +84614,7 @@
         <v>2283</v>
       </c>
       <c r="F1660" s="2"/>
-      <c r="G1660" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1660" s="2"/>
       <c r="H1660" s="2" t="s">
         <v>2174</v>
       </c>
@@ -84857,9 +84663,7 @@
         <v>2284</v>
       </c>
       <c r="F1661" s="2"/>
-      <c r="G1661" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1661" s="2"/>
       <c r="H1661" s="2" t="s">
         <v>2175</v>
       </c>
@@ -84908,9 +84712,7 @@
         <v>2252</v>
       </c>
       <c r="F1662" s="2"/>
-      <c r="G1662" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1662" s="2"/>
       <c r="H1662" s="2" t="s">
         <v>2176</v>
       </c>
@@ -84959,9 +84761,7 @@
         <v>2252</v>
       </c>
       <c r="F1663" s="2"/>
-      <c r="G1663" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1663" s="2"/>
       <c r="H1663" s="2" t="s">
         <v>2158</v>
       </c>
@@ -85010,9 +84810,7 @@
         <v>2285</v>
       </c>
       <c r="F1664" s="2"/>
-      <c r="G1664" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1664" s="2"/>
       <c r="H1664" s="2" t="s">
         <v>2177</v>
       </c>
@@ -85061,9 +84859,7 @@
         <v>2286</v>
       </c>
       <c r="F1665" s="2"/>
-      <c r="G1665" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1665" s="2"/>
       <c r="H1665" s="2" t="s">
         <v>2168</v>
       </c>
@@ -85112,9 +84908,7 @@
         <v>2287</v>
       </c>
       <c r="F1666" s="2"/>
-      <c r="G1666" s="2" t="s">
-        <v>418</v>
-      </c>
+      <c r="G1666" s="2"/>
       <c r="H1666" s="2" t="s">
         <v>2178</v>
       </c>
@@ -87654,12 +87448,20 @@
       <c r="C1731" s="9" t="s">
         <v>2426</v>
       </c>
-      <c r="D1731" s="2"/>
-      <c r="E1731" s="9"/>
+      <c r="D1731" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E1731" s="9" t="s">
+        <v>2427</v>
+      </c>
       <c r="F1731" s="2"/>
       <c r="G1731" s="2"/>
-      <c r="H1731" s="2"/>
-      <c r="I1731" s="2"/>
+      <c r="H1731" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1731" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="J1731" s="12" t="s">
         <v>161</v>
       </c>
@@ -87673,10 +87475,10 @@
       <c r="N1731" s="2"/>
       <c r="O1731" s="2"/>
       <c r="P1731" s="2">
-        <v>45.627220000000001</v>
+        <v>45.625458000000002</v>
       </c>
       <c r="Q1731" s="2">
-        <v>-122.671646</v>
+        <v>-122.674277</v>
       </c>
     </row>
     <row r="1732" spans="1:17" x14ac:dyDescent="0.25">
@@ -87687,13 +87489,13 @@
         <v>2425</v>
       </c>
       <c r="C1732" s="9" t="s">
-        <v>2427</v>
+        <v>2428</v>
       </c>
       <c r="D1732" s="2" t="s">
         <v>401</v>
       </c>
       <c r="E1732" s="9" t="s">
-        <v>2428</v>
+        <v>2429</v>
       </c>
       <c r="F1732" s="2"/>
       <c r="G1732" s="2"/>
@@ -87703,23 +87505,23 @@
       <c r="I1732" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J1732" s="12" t="s">
+      <c r="J1732" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="K1732" s="12" t="s">
+      <c r="K1732" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="L1732" s="12">
+      <c r="L1732" s="2">
         <v>98660</v>
       </c>
       <c r="M1732" s="2"/>
       <c r="N1732" s="2"/>
       <c r="O1732" s="2"/>
       <c r="P1732" s="2">
-        <v>45.625458000000002</v>
+        <v>45.625599999999999</v>
       </c>
       <c r="Q1732" s="2">
-        <v>-122.674277</v>
+        <v>-122.67573899999999</v>
       </c>
     </row>
     <row r="1733" spans="1:17" x14ac:dyDescent="0.25">
@@ -87730,21 +87532,19 @@
         <v>2425</v>
       </c>
       <c r="C1733" s="9" t="s">
-        <v>2429</v>
-      </c>
-      <c r="D1733" s="2" t="s">
-        <v>401</v>
-      </c>
+        <v>2430</v>
+      </c>
+      <c r="D1733" s="2"/>
       <c r="E1733" s="9" t="s">
-        <v>2430</v>
+        <v>2431</v>
       </c>
       <c r="F1733" s="2"/>
       <c r="G1733" s="2"/>
       <c r="H1733" s="2" t="s">
-        <v>44</v>
+        <v>2432</v>
       </c>
       <c r="I1733" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="J1733" s="2" t="s">
         <v>161</v>
@@ -87759,10 +87559,10 @@
       <c r="N1733" s="2"/>
       <c r="O1733" s="2"/>
       <c r="P1733" s="2">
-        <v>45.625599999999999</v>
+        <v>45.623528999999998</v>
       </c>
       <c r="Q1733" s="2">
-        <v>-122.67573899999999</v>
+        <v>-122.674254</v>
       </c>
     </row>
     <row r="1734" spans="1:17" x14ac:dyDescent="0.25">
@@ -87773,16 +87573,18 @@
         <v>2425</v>
       </c>
       <c r="C1734" s="9" t="s">
-        <v>2431</v>
-      </c>
-      <c r="D1734" s="2"/>
+        <v>2433</v>
+      </c>
+      <c r="D1734" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="E1734" s="9" t="s">
-        <v>2432</v>
+        <v>2434</v>
       </c>
       <c r="F1734" s="2"/>
       <c r="G1734" s="2"/>
       <c r="H1734" s="2" t="s">
-        <v>2433</v>
+        <v>397</v>
       </c>
       <c r="I1734" s="2" t="s">
         <v>22</v>
@@ -87800,10 +87602,10 @@
       <c r="N1734" s="2"/>
       <c r="O1734" s="2"/>
       <c r="P1734" s="2">
-        <v>45.623528999999998</v>
+        <v>45.621760000000002</v>
       </c>
       <c r="Q1734" s="2">
-        <v>-122.674254</v>
+        <v>-122.673894</v>
       </c>
     </row>
     <row r="1735" spans="1:17" x14ac:dyDescent="0.25">
@@ -87814,21 +87616,21 @@
         <v>2425</v>
       </c>
       <c r="C1735" s="9" t="s">
-        <v>2434</v>
+        <v>2435</v>
       </c>
       <c r="D1735" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E1735" s="9" t="s">
-        <v>2435</v>
+        <v>2437</v>
       </c>
       <c r="F1735" s="2"/>
       <c r="G1735" s="2"/>
       <c r="H1735" s="2" t="s">
-        <v>397</v>
+        <v>1063</v>
       </c>
       <c r="I1735" s="2" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="J1735" s="2" t="s">
         <v>161</v>
@@ -87837,16 +87639,16 @@
         <v>162</v>
       </c>
       <c r="L1735" s="2">
-        <v>98660</v>
+        <v>98661</v>
       </c>
       <c r="M1735" s="2"/>
       <c r="N1735" s="2"/>
       <c r="O1735" s="2"/>
       <c r="P1735" s="2">
-        <v>45.621760000000002</v>
+        <v>45.615172000000001</v>
       </c>
       <c r="Q1735" s="2">
-        <v>-122.673894</v>
+        <v>-122.652911</v>
       </c>
     </row>
     <row r="1736" spans="1:17" x14ac:dyDescent="0.25">
@@ -87859,19 +87661,17 @@
       <c r="C1736" s="9" t="s">
         <v>2436</v>
       </c>
-      <c r="D1736" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="D1736" s="2"/>
       <c r="E1736" s="9" t="s">
-        <v>2438</v>
+        <v>2185</v>
       </c>
       <c r="F1736" s="2"/>
       <c r="G1736" s="2"/>
       <c r="H1736" s="2" t="s">
-        <v>1063</v>
+        <v>354</v>
       </c>
       <c r="I1736" s="2" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="J1736" s="2" t="s">
         <v>161</v>
@@ -87886,10 +87686,10 @@
       <c r="N1736" s="2"/>
       <c r="O1736" s="2"/>
       <c r="P1736" s="2">
-        <v>45.615172000000001</v>
+        <v>45.625090999999998</v>
       </c>
       <c r="Q1736" s="2">
-        <v>-122.652911</v>
+        <v>-122.63919</v>
       </c>
     </row>
     <row r="1737" spans="1:17" x14ac:dyDescent="0.25">
@@ -87900,19 +87700,21 @@
         <v>2425</v>
       </c>
       <c r="C1737" s="9" t="s">
-        <v>2437</v>
-      </c>
-      <c r="D1737" s="2"/>
+        <v>2438</v>
+      </c>
+      <c r="D1737" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="E1737" s="9" t="s">
-        <v>2185</v>
+        <v>2439</v>
       </c>
       <c r="F1737" s="2"/>
       <c r="G1737" s="2"/>
       <c r="H1737" s="2" t="s">
-        <v>354</v>
+        <v>395</v>
       </c>
       <c r="I1737" s="2" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="J1737" s="2" t="s">
         <v>161</v>
@@ -87927,10 +87729,10 @@
       <c r="N1737" s="2"/>
       <c r="O1737" s="2"/>
       <c r="P1737" s="2">
-        <v>45.625090999999998</v>
+        <v>45.631309000000002</v>
       </c>
       <c r="Q1737" s="2">
-        <v>-122.63919</v>
+        <v>-122.648495</v>
       </c>
     </row>
     <row r="1738" spans="1:17" x14ac:dyDescent="0.25">
@@ -87941,21 +87743,19 @@
         <v>2425</v>
       </c>
       <c r="C1738" s="9" t="s">
-        <v>2439</v>
-      </c>
-      <c r="D1738" s="2" t="s">
-        <v>78</v>
-      </c>
+        <v>2440</v>
+      </c>
+      <c r="D1738" s="2"/>
       <c r="E1738" s="9" t="s">
-        <v>2440</v>
+        <v>2441</v>
       </c>
       <c r="F1738" s="2"/>
       <c r="G1738" s="2"/>
       <c r="H1738" s="2" t="s">
-        <v>395</v>
+        <v>2442</v>
       </c>
       <c r="I1738" s="2" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="J1738" s="2" t="s">
         <v>161</v>
@@ -87964,16 +87764,16 @@
         <v>162</v>
       </c>
       <c r="L1738" s="2">
-        <v>98661</v>
+        <v>98663</v>
       </c>
       <c r="M1738" s="2"/>
       <c r="N1738" s="2"/>
       <c r="O1738" s="2"/>
       <c r="P1738" s="2">
-        <v>45.631309000000002</v>
+        <v>45.634577</v>
       </c>
       <c r="Q1738" s="2">
-        <v>-122.648495</v>
+        <v>-122.651753</v>
       </c>
     </row>
     <row r="1739" spans="1:17" x14ac:dyDescent="0.25">
@@ -87983,20 +87783,20 @@
       <c r="B1739" s="12" t="s">
         <v>2425</v>
       </c>
-      <c r="C1739" s="9" t="s">
-        <v>2441</v>
-      </c>
+      <c r="C1739" s="9"/>
       <c r="D1739" s="2"/>
       <c r="E1739" s="9" t="s">
-        <v>2442</v>
+        <v>2443</v>
       </c>
       <c r="F1739" s="2"/>
-      <c r="G1739" s="2"/>
+      <c r="G1739" s="2" t="s">
+        <v>2444</v>
+      </c>
       <c r="H1739" s="2" t="s">
-        <v>2443</v>
+        <v>30</v>
       </c>
       <c r="I1739" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="J1739" s="2" t="s">
         <v>161</v>
@@ -88004,57 +87804,16 @@
       <c r="K1739" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="L1739" s="2">
-        <v>98663</v>
+      <c r="L1739" s="12">
+        <v>98660</v>
       </c>
       <c r="M1739" s="2"/>
       <c r="N1739" s="2"/>
       <c r="O1739" s="2"/>
       <c r="P1739" s="2">
-        <v>45.634577</v>
+        <v>45.627558999999998</v>
       </c>
       <c r="Q1739" s="2">
-        <v>-122.651753</v>
-      </c>
-    </row>
-    <row r="1740" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1740" s="12" t="s">
-        <v>2422</v>
-      </c>
-      <c r="B1740" s="12" t="s">
-        <v>2425</v>
-      </c>
-      <c r="C1740" s="9"/>
-      <c r="D1740" s="2"/>
-      <c r="E1740" s="9" t="s">
-        <v>2444</v>
-      </c>
-      <c r="F1740" s="2"/>
-      <c r="G1740" s="2" t="s">
-        <v>2445</v>
-      </c>
-      <c r="H1740" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1740" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1740" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="K1740" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="L1740" s="12">
-        <v>98660</v>
-      </c>
-      <c r="M1740" s="2"/>
-      <c r="N1740" s="2"/>
-      <c r="O1740" s="2"/>
-      <c r="P1740" s="2">
-        <v>45.627558999999998</v>
-      </c>
-      <c r="Q1740" s="2">
         <v>-122.66968900000001</v>
       </c>
     </row>
@@ -88062,7 +87821,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="E457:E467 E41 E55 E57 E63 E65 E76 E85 E87 E94 E1566:E1572 E1603:E1620 E1583:E1589 E1573:E1582 E1590:E1602 E1634:E1666 E567 E551 E1621:E1633 E1730 E1732:E1733 E1736:E1740" numberStoredAsText="1"/>
+    <ignoredError sqref="E457:E467 E41 E55 E57 E63 E65 E76 E85 E87 E94 E1566:E1572 E1603:E1620 E1583:E1589 E1573:E1582 E1590:E1602 E1634:E1666 E567 E551 E1621:E1633 E1730 E1731:E1732 E1735:E1739" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>